<commit_message>
arbitrary commit. Excel lame.
</commit_message>
<xml_diff>
--- a/PI_all_TM.xlsx
+++ b/PI_all_TM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tristin McHugh\Documents\Github\McHugh-et-al\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88CED6E8-F51D-4CE7-AB14-1740F44419A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07804659-CC69-4E23-84E9-093431FF7DFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{13F64A27-2AF2-C647-87D2-E1E98C450C51}"/>
+    <workbookView xWindow="30000" yWindow="585" windowWidth="17010" windowHeight="9240" xr2:uid="{13F64A27-2AF2-C647-87D2-E1E98C450C51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C231AEC0-29B8-7C44-94BE-EF88D31DABDC}">
   <dimension ref="A1:I961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A944" workbookViewId="0">
-      <selection activeCell="C954" sqref="C954"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>